<commit_message>
Crear validación de horarios en planificacion horaria
Se estructuró la información de la planificación, para facilitar la validación de los horarios, consultando la existencia en la base y si posee detalles registrados para considerar un horario como válido.

Co-Authored-By: Juan Diego <68799845+juandiego-gm@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B87D779-7CEC-B045-8FD9-D862B626E670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6FFF7B-1D90-D846-B490-8F0D20F6E4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,9 +151,6 @@
     <t>1236548952</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>c5</t>
+  </si>
+  <si>
+    <t>C4,JO,UJJ</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,28 +654,28 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="AE2" t="s">
         <v>46</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Verificar sobrexposición de horarios en la plantilla
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6FFF7B-1D90-D846-B490-8F0D20F6E4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D25D393-8C14-574A-8963-4724E17474A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32820" yWindow="2560" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>USUARIO</t>
   </si>
@@ -164,19 +164,39 @@
   </si>
   <si>
     <t>C4,JO,UJJ</t>
+  </si>
+  <si>
+    <t>HR01,HR02</t>
+  </si>
+  <si>
+    <t>HR01,HR-05</t>
+  </si>
+  <si>
+    <t>HR01,HOR-05</t>
+  </si>
+  <si>
+    <t>HOR-05,HOR-05</t>
+  </si>
+  <si>
+    <t>LHORARIO2,HORARIO14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Nunito"/>
     </font>
   </fonts>
   <fills count="2">
@@ -199,8 +219,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +564,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,9 +699,24 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
@@ -731,7 +767,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AF1 A3:AF12 A2 H2:I2 K2:AD2 AF2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:AF1 A4:AF4 A2 H2:I2 K2:AD2 AF2 A6:AF12 A5:B5 D5:AF5 A3 G3:AF3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Verificar sobreposición de horarios en plantilla
Se realiza la verificación de sobreposición de los horarios registrados en la plantilla.
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D25D393-8C14-574A-8963-4724E17474A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5410C991-CEBC-4A44-827E-DFA64FAA08A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32820" yWindow="2560" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>USUARIO</t>
   </si>
@@ -166,9 +166,6 @@
     <t>C4,JO,UJJ</t>
   </si>
   <si>
-    <t>HR01,HR02</t>
-  </si>
-  <si>
     <t>HR01,HR-05</t>
   </si>
   <si>
@@ -179,6 +176,12 @@
   </si>
   <si>
     <t>LHORARIO2,HORARIO14</t>
+  </si>
+  <si>
+    <t>HR01,HR01</t>
+  </si>
+  <si>
+    <t>HR01</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,25 +707,28 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" t="s">
         <v>50</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -767,7 +773,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AF1 A4:AF4 A2 H2:I2 K2:AD2 AF2 A6:AF12 A5:B5 D5:AF5 A3 G3:AF3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D1 A4 A2 H2:I2 K2:AD2 AF2 A6:AF12 A5:B5 D5:AF5 A3 G3:AF3 C4:AF4 F1:AF1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Verificar existencia de feriado
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823EA80C-578D-DF4D-AF2D-B9772398D92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE38465D-53D7-4A4C-8BC7-218A8C6EE507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>USUARIO</t>
   </si>
@@ -564,7 +564,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,6 +689,9 @@
       <c r="F2" t="s">
         <v>17</v>
       </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
       <c r="J2" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Crear componente para visualizar detalle de observaciones
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE38465D-53D7-4A4C-8BC7-218A8C6EE507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CBB559-6701-4645-9930-964974C8B30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>USUARIO</t>
   </si>
@@ -564,7 +564,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,6 +718,9 @@
       <c r="F3" t="s">
         <v>17</v>
       </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -771,7 +774,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A4 A2 H2:I2 K2:AD2 AF2 A6:AF12 A5:B5 D5:AF5 A3 G3:AF3 C4:AF4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A4 A2 H2:I2 L2:AD2 AF2 A6:AF12 A5:B5 D5:AF5 A3 G3:I3 C4:AF4 K3:AF3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificar vista de pagina de carga de plantillas de paginación.
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CBB559-6701-4645-9930-964974C8B30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD37E5-AD6B-874A-95BC-7D7951AC9959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>USUARIO</t>
   </si>
@@ -564,7 +564,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,47 +734,74 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A4 A2 H2:I2 L2:AD2 AF2 A6:AF12 A5:B5 D5:AF5 A3 G3:I3 C4:AF4 K3:AF3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A4 A2 H2:I2 L2:AD2 AF2 A6:B12 A5 E5:AF5 A3 G3:I3 C4:AF4 K3:AF3 D6:AF12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reemplazar planificaciones con errores por valores por defecto, Enviar datos de planificación al servidor.
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD37E5-AD6B-874A-95BC-7D7951AC9959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F14F38-3809-4145-9FE4-67A38E786F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>USUARIO</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>MARTES, 31/10/2023</t>
+  </si>
+  <si>
+    <t>HR-05</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,7 +710,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Registar planificaciones de la plantilla de planificacion multiple en plan general
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F14F38-3809-4145-9FE4-67A38E786F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EBBA17-FFE1-5E4C-B249-D03C0E3B1373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>USUARIO</t>
   </si>
@@ -76,9 +76,6 @@
     <t>LHORARIO2,HORARIO14</t>
   </si>
   <si>
-    <t>HR01,HR01</t>
-  </si>
-  <si>
     <t>HR01</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
   </si>
   <si>
     <t>MARTES, 31/10/2023</t>
-  </si>
-  <si>
-    <t>HR-05</t>
   </si>
 </sst>
 </file>
@@ -567,7 +561,7 @@
   <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,97 +574,97 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>40</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>41</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>48</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>49</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.25">
@@ -678,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -693,7 +687,7 @@
         <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
@@ -706,105 +700,59 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A4 A2 H2:I2 L2:AD2 AF2 A6:B12 A5 E5:AF5 A3 G3:I3 C4:AF4 K3:AF3 D6:AF12" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A4 A2 H2:I2 L2:AD2 AF2 A6:A12 A5 K5:AF5 A3 K4:AF4 K3:AF3 K6:AF12" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificar función para verificar la superposición de los horarios.
Se estructura el código, para abordar los casos completos de superposición y se separa en funciones para mejorar la legibilidad.
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EBBA17-FFE1-5E4C-B249-D03C0E3B1373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1CA86E-670F-7643-9E8E-A18C6DEAD40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-320" yWindow="2780" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,101 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>USUARIO</t>
   </si>
   <si>
+    <t>LUNES, 01/04/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 02/04/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 03/04/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 04/04/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 05/04/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 06/04/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 07/04/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 08/04/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 09/04/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 10/04/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 11/04/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 12/04/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 13/04/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 14/04/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 15/04/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 16/04/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 17/04/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 18/04/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 19/04/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 20/04/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 21/04/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 22/04/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 23/04/2024</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES, 24/04/2024</t>
+  </si>
+  <si>
+    <t>JUEVES, 25/04/2024</t>
+  </si>
+  <si>
+    <t>VIERNES, 26/04/2024</t>
+  </si>
+  <si>
+    <t>SÁBADO, 27/04/2024</t>
+  </si>
+  <si>
+    <t>DOMINGO, 28/04/2024</t>
+  </si>
+  <si>
+    <t>LUNES, 29/04/2024</t>
+  </si>
+  <si>
+    <t>MARTES, 30/04/2024</t>
+  </si>
+  <si>
     <t>1722128905</t>
   </si>
   <si>
@@ -58,125 +148,29 @@
     <t>1236548952</t>
   </si>
   <si>
+    <t>HR01</t>
+  </si>
+  <si>
+    <t>HR01,HR-05</t>
+  </si>
+  <si>
+    <t>HR01,HOR-05</t>
+  </si>
+  <si>
+    <t>HOR-05,HOR-05</t>
+  </si>
+  <si>
     <t>c4</t>
   </si>
   <si>
-    <t>c5</t>
-  </si>
-  <si>
-    <t>HR01,HR-05</t>
-  </si>
-  <si>
-    <t>HR01,HOR-05</t>
-  </si>
-  <si>
-    <t>HOR-05,HOR-05</t>
-  </si>
-  <si>
-    <t>LHORARIO2,HORARIO14</t>
-  </si>
-  <si>
-    <t>HR01</t>
-  </si>
-  <si>
-    <t>DOMINGO, 01/10/2023</t>
-  </si>
-  <si>
-    <t>LUNES, 02/10/2023</t>
-  </si>
-  <si>
-    <t>MARTES, 03/10/2023</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 04/10/2023</t>
-  </si>
-  <si>
-    <t>JUEVES, 05/10/2023</t>
-  </si>
-  <si>
-    <t>VIERNES, 06/10/2023</t>
-  </si>
-  <si>
-    <t>SÁBADO, 07/10/2023</t>
-  </si>
-  <si>
-    <t>DOMINGO, 08/10/2023</t>
-  </si>
-  <si>
-    <t>LUNES, 09/10/2023</t>
-  </si>
-  <si>
-    <t>MARTES, 10/10/2023</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 11/10/2023</t>
-  </si>
-  <si>
-    <t>JUEVES, 12/10/2023</t>
-  </si>
-  <si>
-    <t>VIERNES, 13/10/2023</t>
-  </si>
-  <si>
-    <t>SÁBADO, 14/10/2023</t>
-  </si>
-  <si>
-    <t>DOMINGO, 15/10/2023</t>
-  </si>
-  <si>
-    <t>LUNES, 16/10/2023</t>
-  </si>
-  <si>
-    <t>MARTES, 17/10/2023</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 18/10/2023</t>
-  </si>
-  <si>
-    <t>JUEVES, 19/10/2023</t>
-  </si>
-  <si>
-    <t>VIERNES, 20/10/2023</t>
-  </si>
-  <si>
-    <t>SÁBADO, 21/10/2023</t>
-  </si>
-  <si>
-    <t>DOMINGO, 22/10/2023</t>
-  </si>
-  <si>
-    <t>LUNES, 23/10/2023</t>
-  </si>
-  <si>
-    <t>MARTES, 24/10/2023</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES, 25/10/2023</t>
-  </si>
-  <si>
-    <t>JUEVES, 26/10/2023</t>
-  </si>
-  <si>
-    <t>VIERNES, 27/10/2023</t>
-  </si>
-  <si>
-    <t>SÁBADO, 28/10/2023</t>
-  </si>
-  <si>
-    <t>DOMINGO, 29/10/2023</t>
-  </si>
-  <si>
-    <t>LUNES, 30/10/2023</t>
-  </si>
-  <si>
-    <t>MARTES, 31/10/2023</t>
+    <t>LHORARIO2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,13 +181,8 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Nunito"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Helvetica"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -558,201 +547,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="G8" sqref="G7:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="32" width="20.83203125" customWidth="1"/>
+    <col min="1" max="31" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" t="s">
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="S1" t="s">
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="U1" t="s">
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="W1" t="s">
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="X1" t="s">
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A4 A2 H2:I2 L2:AD2 AF2 A6:A12 A5 K5:AF5 A3 K4:AF4 K3:AF3 K6:AF12" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:AE1 A3:AE12 A2 K2:L2 N2:AE2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificar registro de planificaciones y consulta de planificaciones
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1CA86E-670F-7643-9E8E-A18C6DEAD40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629881C9-A731-D14E-87D2-5F693D9804CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="2780" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35340" yWindow="880" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="53">
   <si>
     <t>USUARIO</t>
   </si>
@@ -164,6 +164,21 @@
   </si>
   <si>
     <t>LHORARIO2</t>
+  </si>
+  <si>
+    <t>HR01, HR02</t>
+  </si>
+  <si>
+    <t>HR01, C4</t>
+  </si>
+  <si>
+    <t>FERIADO 1</t>
+  </si>
+  <si>
+    <t>HR01, FERIADO 1</t>
+  </si>
+  <si>
+    <t>HR01,LHORARIO2</t>
   </si>
 </sst>
 </file>
@@ -550,7 +565,7 @@
   <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G7:G8"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,56 +704,716 @@
       <c r="A3" t="s">
         <v>32</v>
       </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" t="s">
+        <v>42</v>
+      </c>
+      <c r="X5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" t="s">
+        <v>42</v>
+      </c>
+      <c r="W6" t="s">
+        <v>42</v>
+      </c>
+      <c r="X6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>42</v>
+      </c>
+      <c r="R7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" t="s">
+        <v>42</v>
+      </c>
+      <c r="T8" t="s">
+        <v>42</v>
+      </c>
+      <c r="W8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>42</v>
+      </c>
+      <c r="R9" t="s">
+        <v>42</v>
+      </c>
+      <c r="S9" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>42</v>
+      </c>
+      <c r="R10" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" t="s">
+        <v>42</v>
+      </c>
+      <c r="T10" t="s">
+        <v>42</v>
+      </c>
+      <c r="W10" t="s">
+        <v>42</v>
+      </c>
+      <c r="X10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S11" t="s">
+        <v>42</v>
+      </c>
+      <c r="T11" t="s">
+        <v>42</v>
+      </c>
+      <c r="W11" t="s">
+        <v>42</v>
+      </c>
+      <c r="X11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" t="s">
+        <v>42</v>
+      </c>
+      <c r="M12" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R12" t="s">
+        <v>42</v>
+      </c>
+      <c r="S12" t="s">
+        <v>42</v>
+      </c>
+      <c r="T12" t="s">
+        <v>42</v>
+      </c>
+      <c r="W12" t="s">
+        <v>42</v>
+      </c>
+      <c r="X12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AE1 A3:AE12 A2 K2:L2 N2:AE2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:AE1 A5:A12 A2 K2:L2 N2:AE2 A3 G3:H3 A4 N3:O3 U3:V3 AB3:AC3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambiar carga y registro de plantillas horarias
Eliminación en la plantilla de los registro con usuarios no validos antes de registrar, cambio en la forma que se muestran los usuarios no validos, se mantienen en la tabla pero se indica que es no valido y se hace énfasis con un color.

Co-Authored-By: Juan Diego <68799845+juandiego-gm@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000B123D-50BE-6C4F-999C-7104BB12A49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DFE3E3-12CE-1B4C-A7F6-6AC791F83F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Solucionado editar planificacion horaria
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenny\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF03C39A-186C-6449-B6D0-1C055FD0A682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18386D7-BD9F-49B3-9452-B56B20EB1F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36240" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+  <si>
+    <t>EMPLEADO</t>
+  </si>
   <si>
     <t>LUNES, 01/07/2024</t>
   </si>
@@ -115,16 +118,22 @@
     <t>MIÉRCOLES, 31/07/2024</t>
   </si>
   <si>
-    <t>1851841891</t>
-  </si>
-  <si>
-    <t>1759787615</t>
-  </si>
-  <si>
-    <t>OFICINA</t>
-  </si>
-  <si>
-    <t>EMPLEADO</t>
+    <t>1722128905</t>
+  </si>
+  <si>
+    <t>1724157688</t>
+  </si>
+  <si>
+    <t>oficina</t>
+  </si>
+  <si>
+    <t>oficinas</t>
+  </si>
+  <si>
+    <t>pasantia</t>
+  </si>
+  <si>
+    <t>pasantias</t>
   </si>
 </sst>
 </file>
@@ -504,156 +513,264 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="32" width="20.83203125" customWidth="1"/>
+    <col min="1" max="32" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:AF1 A3 A2 G2:AF2 G3:AF3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:AF1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>